<commit_message>
Rimosso nelle colonne Q e R la stringa "FSE"
</commit_message>
<xml_diff>
--- a/Test Case/accreditamento-checklist_V8.2.6.1.xlsx
+++ b/Test Case/accreditamento-checklist_V8.2.6.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irene.stacchiotti\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775FB69C-F117-4E88-BA67-784DF95AE384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A964438-CA3D-403A-94DB-61DD83690133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="975" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33720" yWindow="975" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -1694,9 +1694,6 @@
     <t>8.2.6.1</t>
   </si>
   <si>
-    <t xml:space="preserve"> PRESENTE CODA DI RETRY AUTOMATICA PER L'INVIO DEL DOCUMENTO AL FSE SERVIZIO DI VALIDAZIONE DEL GATEWAY A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)</t>
-  </si>
-  <si>
     <t>Per questo caso di test è richiesta la sola descrizione del comportamento a fronte di un timeout, da inserire nelle colonne relative a:
 "ERRORE BLOCCANTE (SI/NO)", "ERRORE VISIBILE A UTENTE (SI/NO)", "MESSAGGIO DI ERRORE", "GESTITO IN BACKOFFICE (SI/NO)", " PRESENTE CODA DI RETRY AUTOMATICA PER L'INVIO DEL DOCUMENTO AL FSE SERVIZIO DI VALIDAZIONE DEL GATEWAY A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)",  "INVIO MANUALE DEL DOCUMENTO AL FSE A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)", "GESTIONE ERRORE".</t>
   </si>
@@ -1719,7 +1716,10 @@
     GESTIONE ERRORE da compilare con la procedura che viene adottata per la gestione dell'errore, solo per i casi KO (ovvero con CASO OK / KO= KO) e per i casi di test di TIMEOUT,  specificando le modalità di invio del documento clinico al FSE a seguito della correzione dell'errore e chiarendo se è possibile per l'utente (medico) proseguire con il processo e produrre il documento. Esclusivamente per i casi di test di TIMEOUT, qualora non fosse prevista una coda di retry e la gestione dell'errore non fossa gestita da un operatore di backoffice, indicare le modalità attraverso cui è reso esplicito all’utente (medico) di effettuare nuovi tentativi di invio verso il FSE fino al ripristino del servizio di validazione.</t>
   </si>
   <si>
-    <t>INVIO MANUALE DEL DOCUMENTO AL FSE SERVIZIO DI VALIDAZIONE DEL GATEWAY A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)</t>
+    <t>PRESENTE CODA DI RETRY AUTOMATICA PER L'INVIO DEL DOCUMENTO AL SERVIZIO DI VALIDAZIONE DEL GATEWAY A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)</t>
+  </si>
+  <si>
+    <t>INVIO MANUALE DEL DOCUMENTO AL SERVIZIO DI VALIDAZIONE DEL GATEWAY A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)</t>
   </si>
 </sst>
 </file>
@@ -2639,7 +2639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -2671,7 +2671,7 @@
     </row>
     <row r="5" spans="1:1" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="87" x14ac:dyDescent="0.35">
@@ -3787,11 +3787,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W752"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="K10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="M10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="O20" sqref="O20"/>
+      <selection pane="bottomRight" activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4055,7 +4055,7 @@
         <v>31</v>
       </c>
       <c r="Q9" s="20" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="R9" s="20" t="s">
         <v>439</v>
@@ -4719,7 +4719,7 @@
         <v>66</v>
       </c>
       <c r="E27" s="43" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F27" s="37"/>
       <c r="G27" s="37"/>
@@ -4758,7 +4758,7 @@
         <v>68</v>
       </c>
       <c r="E28" s="43" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F28" s="37"/>
       <c r="G28" s="37"/>
@@ -4797,7 +4797,7 @@
         <v>69</v>
       </c>
       <c r="E29" s="43" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F29" s="37"/>
       <c r="G29" s="37"/>
@@ -4836,7 +4836,7 @@
         <v>70</v>
       </c>
       <c r="E30" s="43" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F30" s="37"/>
       <c r="G30" s="37"/>
@@ -4875,7 +4875,7 @@
         <v>71</v>
       </c>
       <c r="E31" s="43" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F31" s="37"/>
       <c r="G31" s="37"/>
@@ -4914,7 +4914,7 @@
         <v>72</v>
       </c>
       <c r="E32" s="43" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F32" s="37"/>
       <c r="G32" s="37"/>
@@ -4953,7 +4953,7 @@
         <v>73</v>
       </c>
       <c r="E33" s="43" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F33" s="37"/>
       <c r="G33" s="37"/>
@@ -4992,7 +4992,7 @@
         <v>74</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="F34" s="37"/>
       <c r="G34" s="37"/>
@@ -9397,7 +9397,7 @@
         <v>255</v>
       </c>
       <c r="E153" s="43" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F153" s="37"/>
       <c r="G153" s="37"/>
@@ -17164,6 +17164,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -17421,28 +17442,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17461,31 +17486,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>